<commit_message>
update the data in Feburary 1st, 2015
</commit_message>
<xml_diff>
--- a/weight_data.xlsx
+++ b/weight_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,10 +151,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$101</c:f>
+              <c:f>Sheet1!$A$2:$A$104</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="103"/>
                 <c:pt idx="0">
                   <c:v>41934.0</c:v>
                 </c:pt>
@@ -454,16 +454,25 @@
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>42033.0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>42034.0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>42035.0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>42036.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$101</c:f>
+              <c:f>Sheet1!$B$2:$B$104</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="103"/>
                 <c:pt idx="0">
                   <c:v>86.7</c:v>
                 </c:pt>
@@ -763,6 +772,15 @@
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>84.8</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>84.6</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>84.5</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>85.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -779,11 +797,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2108489736"/>
-        <c:axId val="2106541192"/>
+        <c:axId val="2083746520"/>
+        <c:axId val="2083749544"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2108489736"/>
+        <c:axId val="2083746520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -793,14 +811,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106541192"/>
+        <c:crossAx val="2083749544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2106541192"/>
+        <c:axId val="2083749544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,7 +829,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108489736"/>
+        <c:crossAx val="2083746520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1155,10 +1173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K73" sqref="K73"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2286,6 +2304,84 @@
     <row r="102" spans="1:3">
       <c r="A102" s="2">
         <v>42034</v>
+      </c>
+      <c r="B102" s="1">
+        <v>84.6</v>
+      </c>
+      <c r="C102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="2">
+        <v>42035</v>
+      </c>
+      <c r="B103" s="1">
+        <v>84.5</v>
+      </c>
+      <c r="C103" s="1">
+        <v>10.51</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="2">
+        <v>42036</v>
+      </c>
+      <c r="B104" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="2">
+        <v>42037</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="2">
+        <v>42038</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="2">
+        <v>42039</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="2">
+        <v>42040</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="2">
+        <v>42041</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="2">
+        <v>42042</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="2">
+        <v>42043</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="2">
+        <v>42044</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="2">
+        <v>42045</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="2">
+        <v>42046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the data in February 17th
</commit_message>
<xml_diff>
--- a/weight_data.xlsx
+++ b/weight_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,10 +151,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$104</c:f>
+              <c:f>Sheet1!$A$2:$A$120</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="119"/>
                 <c:pt idx="0">
                   <c:v>41934.0</c:v>
                 </c:pt>
@@ -463,16 +463,64 @@
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>42036.0</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>42037.0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>42038.0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>42039.0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>42040.0</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>42041.0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>42042.0</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>42043.0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>42044.0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>42045.0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>42046.0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>42047.0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>42048.0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>42049.0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>42050.0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>42051.0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>42052.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$104</c:f>
+              <c:f>Sheet1!$B$2:$B$120</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="103"/>
+                <c:ptCount val="119"/>
                 <c:pt idx="0">
                   <c:v>86.7</c:v>
                 </c:pt>
@@ -780,6 +828,54 @@
                   <c:v>84.5</c:v>
                 </c:pt>
                 <c:pt idx="102">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>86.4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>85.9</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>85.1</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>83.7</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>85.9</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>85.6</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>85.5</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>85.7</c:v>
+                </c:pt>
+                <c:pt idx="118">
                   <c:v>85.2</c:v>
                 </c:pt>
               </c:numCache>
@@ -797,11 +893,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2083746520"/>
-        <c:axId val="2083749544"/>
+        <c:axId val="2108002792"/>
+        <c:axId val="2109090376"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2083746520"/>
+        <c:axId val="2108002792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -811,14 +907,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083749544"/>
+        <c:crossAx val="2109090376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2083749544"/>
+        <c:axId val="2109090376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,7 +925,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2083746520"/>
+        <c:crossAx val="2108002792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1173,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2338,50 +2434,176 @@
       <c r="A105" s="2">
         <v>42037</v>
       </c>
+      <c r="B105" s="1">
+        <v>86.4</v>
+      </c>
+      <c r="C105" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="2">
         <v>42038</v>
       </c>
+      <c r="B106" s="1">
+        <v>85.9</v>
+      </c>
+      <c r="C106" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="2">
         <v>42039</v>
       </c>
+      <c r="B107" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C107" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="2">
         <v>42040</v>
       </c>
+      <c r="B108" s="1">
+        <v>85.1</v>
+      </c>
+      <c r="C108" s="1">
+        <v>5.61</v>
+      </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="2">
         <v>42041</v>
       </c>
+      <c r="B109" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C109" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="2">
         <v>42042</v>
       </c>
+      <c r="B110" s="1">
+        <v>83.7</v>
+      </c>
+      <c r="C110" s="1">
+        <v>21.11</v>
+      </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="2">
         <v>42043</v>
       </c>
+      <c r="B111" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C111" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="2">
         <v>42044</v>
       </c>
-    </row>
-    <row r="113" spans="1:1">
+      <c r="B112" s="1">
+        <v>85.9</v>
+      </c>
+      <c r="C112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
       <c r="A113" s="2">
         <v>42045</v>
       </c>
-    </row>
-    <row r="114" spans="1:1">
+      <c r="B113" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C113" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
       <c r="A114" s="2">
         <v>42046</v>
+      </c>
+      <c r="B114" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C114" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="2">
+        <v>42047</v>
+      </c>
+      <c r="B115" s="1">
+        <v>85.6</v>
+      </c>
+      <c r="C115" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="2">
+        <v>42048</v>
+      </c>
+      <c r="B116" s="1">
+        <v>85.5</v>
+      </c>
+      <c r="C116" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="2">
+        <v>42049</v>
+      </c>
+      <c r="B117" s="1">
+        <v>85</v>
+      </c>
+      <c r="C117" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="2">
+        <v>42050</v>
+      </c>
+      <c r="B118" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C118" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="2">
+        <v>42051</v>
+      </c>
+      <c r="B119" s="1">
+        <v>85.7</v>
+      </c>
+      <c r="C119" s="1">
+        <v>6.12</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="2">
+        <v>42052</v>
+      </c>
+      <c r="B120" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C120" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data in March 8th, 2015
</commit_message>
<xml_diff>
--- a/weight_data.xlsx
+++ b/weight_data.xlsx
@@ -151,10 +151,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$120</c:f>
+              <c:f>Sheet1!$A$2:$A$139</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="119"/>
+                <c:ptCount val="138"/>
                 <c:pt idx="0">
                   <c:v>41934.0</c:v>
                 </c:pt>
@@ -511,16 +511,73 @@
                 </c:pt>
                 <c:pt idx="118">
                   <c:v>42052.0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42053.0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>42054.0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>42055.0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>42056.0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>42057.0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>42058.0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>42059.0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>42060.0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>42061.0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>42062.0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>42063.0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>42064.0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>42065.0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>42066.0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>42067.0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>42068.0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>42069.0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>42070.0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>42071.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$120</c:f>
+              <c:f>Sheet1!$B$2:$B$139</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="119"/>
+                <c:ptCount val="138"/>
                 <c:pt idx="0">
                   <c:v>86.7</c:v>
                 </c:pt>
@@ -877,6 +934,63 @@
                 </c:pt>
                 <c:pt idx="118">
                   <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>86.5</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>86.2</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>85.7</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>85.8</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>85.5</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>85.7</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>86.1</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>86.6</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>86.9</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>85.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -893,11 +1007,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2108002792"/>
-        <c:axId val="2109090376"/>
+        <c:axId val="2101053496"/>
+        <c:axId val="2101057016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2108002792"/>
+        <c:axId val="2101053496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -907,14 +1021,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109090376"/>
+        <c:crossAx val="2101057016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2109090376"/>
+        <c:axId val="2101057016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -925,7 +1039,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108002792"/>
+        <c:crossAx val="2101053496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1269,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
+      <selection activeCell="C139" sqref="C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2604,6 +2718,215 @@
       </c>
       <c r="C120" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="2">
+        <v>42053</v>
+      </c>
+      <c r="B121" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="C121" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="2">
+        <v>42054</v>
+      </c>
+      <c r="B122" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="C122" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="2">
+        <v>42055</v>
+      </c>
+      <c r="B123" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="C123" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="2">
+        <v>42056</v>
+      </c>
+      <c r="B124" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="C124" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="2">
+        <v>42057</v>
+      </c>
+      <c r="B125" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="C125" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="2">
+        <v>42058</v>
+      </c>
+      <c r="B126" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="C126" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="2">
+        <v>42059</v>
+      </c>
+      <c r="B127" s="1">
+        <v>86.5</v>
+      </c>
+      <c r="C127" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="2">
+        <v>42060</v>
+      </c>
+      <c r="B128" s="1">
+        <v>86.2</v>
+      </c>
+      <c r="C128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="2">
+        <v>42061</v>
+      </c>
+      <c r="B129" s="1">
+        <v>85.7</v>
+      </c>
+      <c r="C129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="2">
+        <v>42062</v>
+      </c>
+      <c r="B130" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C130" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="2">
+        <v>42063</v>
+      </c>
+      <c r="B131" s="1">
+        <v>85.4</v>
+      </c>
+      <c r="C131" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="2">
+        <v>42064</v>
+      </c>
+      <c r="B132" s="1">
+        <v>85.8</v>
+      </c>
+      <c r="C132" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="2">
+        <v>42065</v>
+      </c>
+      <c r="B133" s="1">
+        <v>85.5</v>
+      </c>
+      <c r="C133" s="1">
+        <v>7.02</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="2">
+        <v>42066</v>
+      </c>
+      <c r="B134" s="1">
+        <v>85</v>
+      </c>
+      <c r="C134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="2">
+        <v>42067</v>
+      </c>
+      <c r="B135" s="1">
+        <v>85.7</v>
+      </c>
+      <c r="C135" s="1">
+        <v>8.51</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="2">
+        <v>42068</v>
+      </c>
+      <c r="B136" s="1">
+        <v>86.1</v>
+      </c>
+      <c r="C136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="2">
+        <v>42069</v>
+      </c>
+      <c r="B137" s="1">
+        <v>86.6</v>
+      </c>
+      <c r="C137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="2">
+        <v>42070</v>
+      </c>
+      <c r="B138" s="1">
+        <v>86.9</v>
+      </c>
+      <c r="C138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="2">
+        <v>42071</v>
+      </c>
+      <c r="B139" s="1">
+        <v>85</v>
+      </c>
+      <c r="C139" s="1">
+        <v>10.11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update weight data in April 21th
</commit_message>
<xml_diff>
--- a/weight_data.xlsx
+++ b/weight_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="24709"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,10 +151,10 @@
           </c:tx>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$139</c:f>
+              <c:f>Sheet1!$A$2:$A$183</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="138"/>
+                <c:ptCount val="182"/>
                 <c:pt idx="0">
                   <c:v>41934.0</c:v>
                 </c:pt>
@@ -568,16 +568,148 @@
                 </c:pt>
                 <c:pt idx="137">
                   <c:v>42071.0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>42072.0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>42073.0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>42074.0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>42075.0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>42076.0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>42077.0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>42078.0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>42079.0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>42080.0</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>42081.0</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>42082.0</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>42083.0</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>42084.0</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>42085.0</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>42086.0</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>42087.0</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>42088.0</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>42089.0</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>42090.0</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>42091.0</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>42092.0</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>42093.0</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>42094.0</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>42095.0</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>42096.0</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>42097.0</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>42098.0</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>42099.0</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>42100.0</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>42101.0</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>42102.0</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>42103.0</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>42104.0</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>42105.0</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>42106.0</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>42107.0</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>42108.0</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>42109.0</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>42110.0</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>42111.0</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>42112.0</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>42113.0</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>42114.0</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>42115.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$139</c:f>
+              <c:f>Sheet1!$B$2:$B$183</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="138"/>
+                <c:ptCount val="182"/>
                 <c:pt idx="0">
                   <c:v>86.7</c:v>
                 </c:pt>
@@ -991,6 +1123,138 @@
                 </c:pt>
                 <c:pt idx="137">
                   <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>85.3</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>85.6</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>85.6</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>85.3</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>84.6</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>86.4</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>85.7</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>86.1</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>84.6</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>85.8</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>84.3</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>84.6</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>84.6</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>85.7</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>85.6</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>84.7</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>84.3</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>83.9</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>83.0</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>85.3</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>85.3</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>84.5</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>83.5</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>84.3</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>84.5</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>85.1</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>84.4</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>84.8</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>83.2</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>83.0</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>84.1</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>83.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1007,11 +1271,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2101053496"/>
-        <c:axId val="2101057016"/>
+        <c:axId val="2109378744"/>
+        <c:axId val="2109381672"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2101053496"/>
+        <c:axId val="2109378744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,14 +1285,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101057016"/>
+        <c:crossAx val="2109381672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2101057016"/>
+        <c:axId val="2109381672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1039,7 +1303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2101053496"/>
+        <c:crossAx val="2109378744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1383,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D139"/>
+  <dimension ref="A1:D183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C139" sqref="C139"/>
+    <sheetView tabSelected="1" topLeftCell="D28" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2927,6 +3191,490 @@
       </c>
       <c r="C139" s="1">
         <v>10.11</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="2">
+        <v>42072</v>
+      </c>
+      <c r="B140" s="1">
+        <v>85.3</v>
+      </c>
+      <c r="C140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="2">
+        <v>42073</v>
+      </c>
+      <c r="B141" s="1">
+        <v>85.6</v>
+      </c>
+      <c r="C141" s="1">
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="2">
+        <v>42074</v>
+      </c>
+      <c r="B142" s="1">
+        <v>85.6</v>
+      </c>
+      <c r="C142" s="1">
+        <v>7.11</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="2">
+        <v>42075</v>
+      </c>
+      <c r="B143" s="1">
+        <v>85.4</v>
+      </c>
+      <c r="C143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="2">
+        <v>42076</v>
+      </c>
+      <c r="B144" s="1">
+        <v>85.3</v>
+      </c>
+      <c r="C144" s="1">
+        <v>12.04</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="2">
+        <v>42077</v>
+      </c>
+      <c r="B145" s="1">
+        <v>84.6</v>
+      </c>
+      <c r="C145" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="2">
+        <v>42078</v>
+      </c>
+      <c r="B146" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C146" s="1">
+        <v>30.13</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="2">
+        <v>42079</v>
+      </c>
+      <c r="B147" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C147" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="2">
+        <v>42080</v>
+      </c>
+      <c r="B148" s="1">
+        <v>86.4</v>
+      </c>
+      <c r="C148" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="2">
+        <v>42081</v>
+      </c>
+      <c r="B149" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C149" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="2">
+        <v>42082</v>
+      </c>
+      <c r="B150" s="1">
+        <v>85.7</v>
+      </c>
+      <c r="C150" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="2">
+        <v>42083</v>
+      </c>
+      <c r="B151" s="1">
+        <v>86.1</v>
+      </c>
+      <c r="C151" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="2">
+        <v>42084</v>
+      </c>
+      <c r="B152" s="1">
+        <v>84.6</v>
+      </c>
+      <c r="C152" s="1">
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="2">
+        <v>42085</v>
+      </c>
+      <c r="B153" s="1">
+        <v>85.8</v>
+      </c>
+      <c r="C153" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="2">
+        <v>42086</v>
+      </c>
+      <c r="B154" s="1">
+        <v>84.3</v>
+      </c>
+      <c r="C154" s="1">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="2">
+        <v>42087</v>
+      </c>
+      <c r="B155" s="1">
+        <v>85</v>
+      </c>
+      <c r="C155" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="2">
+        <v>42088</v>
+      </c>
+      <c r="B156" s="1">
+        <v>84.6</v>
+      </c>
+      <c r="C156" s="1">
+        <v>12.14</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="2">
+        <v>42089</v>
+      </c>
+      <c r="B157" s="1">
+        <v>84.6</v>
+      </c>
+      <c r="C157" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="2">
+        <v>42090</v>
+      </c>
+      <c r="B158" s="1">
+        <v>86</v>
+      </c>
+      <c r="C158" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="2">
+        <v>42091</v>
+      </c>
+      <c r="B159" s="1">
+        <v>85.7</v>
+      </c>
+      <c r="C159" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="2">
+        <v>42092</v>
+      </c>
+      <c r="B160" s="1">
+        <v>85.4</v>
+      </c>
+      <c r="C160" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="2">
+        <v>42093</v>
+      </c>
+      <c r="B161" s="1">
+        <v>85.4</v>
+      </c>
+      <c r="C161" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="2">
+        <v>42094</v>
+      </c>
+      <c r="B162" s="1">
+        <v>85.6</v>
+      </c>
+      <c r="C162" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="2">
+        <v>42095</v>
+      </c>
+      <c r="B163" s="1">
+        <v>85.4</v>
+      </c>
+      <c r="C163" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="2">
+        <v>42096</v>
+      </c>
+      <c r="B164" s="1">
+        <v>84.7</v>
+      </c>
+      <c r="C164" s="1">
+        <v>5.31</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="2">
+        <v>42097</v>
+      </c>
+      <c r="B165" s="1">
+        <v>84.3</v>
+      </c>
+      <c r="C165" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="2">
+        <v>42098</v>
+      </c>
+      <c r="B166" s="1">
+        <v>83.9</v>
+      </c>
+      <c r="C166" s="1">
+        <v>32.14</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="2">
+        <v>42099</v>
+      </c>
+      <c r="B167" s="1">
+        <v>83</v>
+      </c>
+      <c r="C167" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="2">
+        <v>42100</v>
+      </c>
+      <c r="B168" s="1">
+        <v>85.3</v>
+      </c>
+      <c r="C168" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="2">
+        <v>42101</v>
+      </c>
+      <c r="B169" s="1">
+        <v>85.3</v>
+      </c>
+      <c r="C169" s="1">
+        <v>7.52</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="2">
+        <v>42102</v>
+      </c>
+      <c r="B170" s="1">
+        <v>84.5</v>
+      </c>
+      <c r="C170" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" s="2">
+        <v>42103</v>
+      </c>
+      <c r="B171" s="1">
+        <v>83.5</v>
+      </c>
+      <c r="C171" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="2">
+        <v>42104</v>
+      </c>
+      <c r="B172" s="1">
+        <v>84.3</v>
+      </c>
+      <c r="C172" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="2">
+        <v>42105</v>
+      </c>
+      <c r="B173" s="1">
+        <v>85.2</v>
+      </c>
+      <c r="C173" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" s="2">
+        <v>42106</v>
+      </c>
+      <c r="B174" s="1">
+        <v>84.5</v>
+      </c>
+      <c r="C174" s="1">
+        <v>12.02</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" s="2">
+        <v>42107</v>
+      </c>
+      <c r="B175" s="1">
+        <v>85.1</v>
+      </c>
+      <c r="C175" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="2">
+        <v>42108</v>
+      </c>
+      <c r="B176" s="1">
+        <v>84.4</v>
+      </c>
+      <c r="C176" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="2">
+        <v>42109</v>
+      </c>
+      <c r="B177" s="1">
+        <v>84.8</v>
+      </c>
+      <c r="C177" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="2">
+        <v>42110</v>
+      </c>
+      <c r="B178" s="1">
+        <v>84</v>
+      </c>
+      <c r="C178" s="1">
+        <v>11.34</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" s="2">
+        <v>42111</v>
+      </c>
+      <c r="B179" s="1">
+        <v>83.2</v>
+      </c>
+      <c r="C179" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="2">
+        <v>42112</v>
+      </c>
+      <c r="B180" s="1">
+        <v>84</v>
+      </c>
+      <c r="C180" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="2">
+        <v>42113</v>
+      </c>
+      <c r="B181" s="1">
+        <v>83</v>
+      </c>
+      <c r="C181" s="1">
+        <v>18.04</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="2">
+        <v>42114</v>
+      </c>
+      <c r="B182" s="1">
+        <v>84.1</v>
+      </c>
+      <c r="C182" s="1">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" s="2">
+        <v>42115</v>
+      </c>
+      <c r="B183" s="1">
+        <v>83.9</v>
+      </c>
+      <c r="C183" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>